<commit_message>
Discussion: appearance + minor updates other results
</commit_message>
<xml_diff>
--- a/data/discussion/3_sparsify.xlsx
+++ b/data/discussion/3_sparsify.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sousa\Dev\slr-ltlm-mr\data\discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDFF818-C220-4C31-B662-2D3BB4A96417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C58537-D7E4-4D10-99FD-6AC592BBD9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="321">
   <si>
     <t>old notes</t>
   </si>
@@ -480,9 +480,6 @@
   </si>
   <si>
     <t>remove STM features based on observability feature strength</t>
-  </si>
-  <si>
-    <t>#observations ~ feature strength</t>
   </si>
   <si>
     <t>removing useless features avoid ever-increasing #features</t>
@@ -1004,6 +1001,12 @@
   </si>
   <si>
     <t>select most representative keyframes using DBSCAN for topic space clustering</t>
+  </si>
+  <si>
+    <t>remove STM features based on information feature strength</t>
+  </si>
+  <si>
+    <t>feature strength ~ information content by sum of reciprocals of main diagonal elements of covariance matrix</t>
   </si>
 </sst>
 </file>
@@ -1359,15 +1362,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="20.77734375" style="4"/>
+    <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="20.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="2" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="193.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" ht="247.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1650,7 +1653,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1685,115 +1688,115 @@
         <v>139</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>146</v>
+        <v>319</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>139</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y3" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z3" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="Z3" s="4" t="s">
-        <v>212</v>
-      </c>
       <c r="AA3" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AD3" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AG3" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH3" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="AH3" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="AI3" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AL3" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AM3" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AN3" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="AO3" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="AO3" s="4" t="s">
-        <v>284</v>
-      </c>
       <c r="AP3" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AQ3" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AR3" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AS3" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AT3" s="4" t="s">
         <v>93</v>
       </c>
       <c r="AU3" s="4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" ht="122.4" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>95</v>
       </c>
@@ -1828,109 +1831,109 @@
         <v>143</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z4" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AD4" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AE4" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AF4" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AH4" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AI4" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AJ4" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AL4" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AM4" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AN4" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AO4" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AP4" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AQ4" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AR4" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AS4" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AU4" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" ht="91.8" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" ht="101.25" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>97</v>
       </c>
@@ -1965,100 +1968,100 @@
         <v>144</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q5" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="R5" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="S5" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AI5" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AL5" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AM5" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AN5" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AP5" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AQ5" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AR5" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AS5" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AU5" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" ht="112.2" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" ht="135" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>98</v>
       </c>
@@ -2090,89 +2093,89 @@
         <v>145</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>63</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF6" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AG6" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AH6" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AI6" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AK6" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL6" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AM6" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AP6" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AR6" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AS6" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AU6" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" ht="102" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" ht="123.75" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>100</v>
       </c>
@@ -2189,80 +2192,80 @@
         <v>131</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>147</v>
+        <v>320</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF7" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AG7" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AH7" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AI7" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AL7" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AP7" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AR7" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AS7" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" ht="71.400000000000006" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="78.75" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>104</v>
       </c>
@@ -2276,45 +2279,45 @@
         <v>130</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AG8" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AH8" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AI8" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AR8" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AS8" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" ht="51" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" ht="56.25" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>111</v>
@@ -2323,10 +2326,10 @@
         <v>123</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" ht="51" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" ht="67.5" x14ac:dyDescent="0.25">
       <c r="G10" s="4" t="s">
         <v>125</v>
       </c>
@@ -2341,11 +2344,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC6CFD6-58EC-408B-BAE2-ED624577AB64}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2353,7 +2356,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2361,78 +2364,78 @@
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>220</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>284</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>310</v>
-      </c>
-    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>96</v>
+      <c r="A12" s="5" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>109</v>
@@ -2440,18 +2443,18 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2459,7 +2462,7 @@
         <v>22</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2467,7 +2470,7 @@
         <v>34</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2475,12 +2478,12 @@
         <v>38</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,7 +2491,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2496,7 +2499,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2504,7 +2507,7 @@
         <v>27</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2512,12 +2515,12 @@
         <v>36</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2525,7 +2528,7 @@
         <v>15</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2533,7 +2536,7 @@
         <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2541,12 +2544,12 @@
         <v>45</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2586,7 +2589,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2602,7 +2605,7 @@
         <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2610,7 +2613,7 @@
         <v>20</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2618,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2626,7 +2629,7 @@
         <v>26</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2634,7 +2637,7 @@
         <v>29</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2642,7 +2645,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2650,7 +2653,7 @@
         <v>35</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2658,12 +2661,12 @@
         <v>42</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2679,7 +2682,7 @@
         <v>13</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2687,7 +2690,7 @@
         <v>32</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2695,7 +2698,7 @@
         <v>33</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2703,7 +2706,7 @@
         <v>37</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2711,12 +2714,12 @@
         <v>40</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2724,7 +2727,7 @@
         <v>18</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2732,7 +2735,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2756,7 +2759,7 @@
         <v>21</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2764,7 +2767,7 @@
         <v>22</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2772,7 +2775,7 @@
         <v>31</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2780,7 +2783,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2788,7 +2791,7 @@
         <v>39</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2796,7 +2799,7 @@
         <v>47</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Discussion (article): appearance > experience maps + illumination transformations + handcrafted features
</commit_message>
<xml_diff>
--- a/data/discussion/3_sparsify.xlsx
+++ b/data/discussion/3_sparsify.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sousa\Dev\slr-ltlm-mr\data\discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C58537-D7E4-4D10-99FD-6AC592BBD9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069244F8-7862-40B9-96D7-BFF313BDAC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19245" yWindow="4980" windowWidth="16200" windowHeight="9210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -1013,7 +1013,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1033,6 +1033,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1362,15 +1368,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="20.7109375" style="4"/>
+    <col min="1" max="1" width="10.6640625" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="20.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" s="2" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="247.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" ht="193.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1653,7 +1659,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" ht="122.4" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>95</v>
       </c>
@@ -1933,7 +1939,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:47" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" ht="91.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>97</v>
       </c>
@@ -2061,7 +2067,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:47" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" ht="112.2" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>98</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:47" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" ht="102" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>100</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:47" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>104</v>
       </c>
@@ -2315,7 +2321,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:47" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" ht="51" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
         <v>216</v>
       </c>
@@ -2329,7 +2335,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="10" spans="1:47" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" ht="51" x14ac:dyDescent="0.3">
       <c r="G10" s="4" t="s">
         <v>125</v>
       </c>
@@ -2344,11 +2350,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC6CFD6-58EC-408B-BAE2-ED624577AB64}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2803,6 +2811,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Discussion: map sparsification (draft)
</commit_message>
<xml_diff>
--- a/data/discussion/3_sparsify.xlsx
+++ b/data/discussion/3_sparsify.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sousa\Dev\slr-ltlm-mr\data\discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AA3B08-7989-42F4-A10B-EF1F07E8C6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4D2BA5-5AF6-4715-96FB-EC572AEC066B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24552" yWindow="1032" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
     <sheet name="organization" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="325">
   <si>
     <t>old notes</t>
   </si>
@@ -1013,6 +1014,12 @@
   </si>
   <si>
     <t>concentratio ratio + track length to determine if add point or not | rmv features in highly dense areas</t>
+  </si>
+  <si>
+    <t>sum over the qualities of the observed LLamas in a frame must be higher than a quality threshold for its addition into the map</t>
+  </si>
+  <si>
+    <t>remove redundant keyframes from the graph without performing any marginalization</t>
   </si>
 </sst>
 </file>
@@ -1047,12 +1054,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1067,7 +1080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,17 +1090,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1371,7 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2083,7 +2103,7 @@
       <c r="F6" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>121</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -2279,7 +2299,7 @@
       <c r="D8" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>124</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -2349,11 +2369,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC6CFD6-58EC-408B-BAE2-ED624577AB64}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView topLeftCell="A52" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2361,7 +2379,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2369,20 +2387,23 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>205</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -2390,432 +2411,466 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>28</v>
+      <c r="A6" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>30</v>
+      <c r="A7" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>41</v>
+      <c r="A8" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>43</v>
+      <c r="A9" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>290</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>93</v>
+      <c r="A10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>309</v>
+      <c r="A12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>2</v>
+      <c r="A13" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>4</v>
+      <c r="A14" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>5</v>
+      <c r="A15" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>8</v>
+      <c r="A16" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>131</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>22</v>
+      <c r="A17" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>34</v>
+      <c r="A18" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>271</v>
+      <c r="A19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>310</v>
+      <c r="A21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>21</v>
+      <c r="A22" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>23</v>
+      <c r="A23" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>27</v>
+      <c r="A24" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>36</v>
+      <c r="A25" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>261</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>322</v>
+      <c r="A26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>311</v>
+      <c r="A28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>15</v>
+      <c r="A29" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>162</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
+      <c r="A30" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>299</v>
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>314</v>
+      <c r="A33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>6</v>
+      <c r="A34" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>7</v>
+      <c r="A35" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>10</v>
+      <c r="A36" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>11</v>
+      <c r="A37" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>17</v>
+      <c r="A39" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>19</v>
+      <c r="A40" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>20</v>
+      <c r="A41" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>25</v>
+      <c r="A42" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>26</v>
+      <c r="A43" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>225</v>
-      </c>
+      <c r="A44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
+      <c r="A45" s="8" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
-        <v>315</v>
+      <c r="A46" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
-        <v>35</v>
+      <c r="A47" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>285</v>
+      <c r="A48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
-        <v>313</v>
+      <c r="A50" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
-        <v>9</v>
+      <c r="A51" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
-        <v>13</v>
+      <c r="A52" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>148</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
-        <v>32</v>
+      <c r="A53" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
-        <v>33</v>
+      <c r="A54" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
-        <v>37</v>
+      <c r="A55" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>282</v>
+      <c r="A56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>312</v>
+      <c r="A58" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>318</v>
+      <c r="A59" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="11" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="5"/>
+      <c r="A60" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="11" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F64" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F65" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="8"/>
+      <c r="A67" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="10"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="8" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="8" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>305</v>
       </c>
     </row>

</xml_diff>